<commit_message>
edits to tests: added Settings.Set Engine option to excel file. Added more validations.
</commit_message>
<xml_diff>
--- a/tests/end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31014A11-1D06-4475-8CD9-CC81BB29D241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C162C4-EA06-4A46-94CD-25D616A834B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
     <sheet name="crediti a inizi 2023" sheetId="2" r:id="rId2"/>
     <sheet name="debiti a inizi 2023" sheetId="3" r:id="rId3"/>
+    <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'costi e ricavi simulazione'!$A$5:$D$110</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="460">
   <si>
     <t>costi acquisti [fissi]</t>
   </si>
@@ -1418,6 +1419,27 @@
   <si>
     <t>$$ tab Set</t>
   </si>
+  <si>
+    <t>$$ mod Settings.Set</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>$engine</t>
+  </si>
+  <si>
+    <t>https://github.com/77it/financial-modeling/blob/master/src/engine/engine.js</t>
+  </si>
 </sst>
 </file>
 
@@ -1428,7 +1450,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1542,8 +1564,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1598,8 +1636,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1651,16 +1701,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1761,12 +1836,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" xfId="6" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{274F127A-7C8C-43C7-A4CF-3934B66104B5}"/>
     <cellStyle name="Comma 2 2" xfId="4" xr:uid="{08036167-C79C-4A1F-822B-535A1632E488}"/>
     <cellStyle name="Comma 2 3" xfId="2" xr:uid="{D614F647-4E31-4F6F-A208-E19F25DAA59C}"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3234,7 +3319,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3248,23 +3333,23 @@
   <dimension ref="A1:CM110"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="4" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" style="4" customWidth="1"/>
-    <col min="9" max="18" width="8.81640625" style="2" customWidth="1"/>
-    <col min="19" max="103" width="20.54296875" style="2" customWidth="1"/>
-    <col min="104" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="2" width="20.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="8.77734375" style="4" customWidth="1"/>
+    <col min="9" max="18" width="8.77734375" style="2" customWidth="1"/>
+    <col min="19" max="103" width="20.5546875" style="2" customWidth="1"/>
+    <col min="104" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:91" ht="63" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:91" ht="63" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -3354,13 +3439,13 @@
       <c r="CL1"/>
       <c r="CM1"/>
     </row>
-    <row r="3" spans="1:91" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:91" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:91" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:91" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -3416,7 +3501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>92</v>
       </c>
@@ -3466,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>92</v>
       </c>
@@ -3516,7 +3601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>92</v>
       </c>
@@ -3566,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>92</v>
       </c>
@@ -3616,7 +3701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>90</v>
       </c>
@@ -3666,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>90</v>
       </c>
@@ -3716,7 +3801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>91</v>
       </c>
@@ -3766,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>91</v>
       </c>
@@ -3816,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>0</v>
       </c>
@@ -3870,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>0</v>
       </c>
@@ -3924,7 +4009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>0</v>
       </c>
@@ -3978,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>0</v>
       </c>
@@ -4032,7 +4117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>0</v>
       </c>
@@ -4086,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>0</v>
       </c>
@@ -4140,7 +4225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>0</v>
       </c>
@@ -4194,7 +4279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>0</v>
       </c>
@@ -4248,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>0</v>
       </c>
@@ -4356,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>0</v>
       </c>
@@ -4410,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>0</v>
       </c>
@@ -4464,7 +4549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>0</v>
       </c>
@@ -4518,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>0</v>
       </c>
@@ -4572,7 +4657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>0</v>
       </c>
@@ -4626,7 +4711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>0</v>
       </c>
@@ -4680,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>0</v>
       </c>
@@ -4734,7 +4819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>1</v>
       </c>
@@ -4790,7 +4875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>1</v>
       </c>
@@ -4846,7 +4931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>1</v>
       </c>
@@ -4900,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>1</v>
       </c>
@@ -4954,7 +5039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>1</v>
       </c>
@@ -5008,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>1</v>
       </c>
@@ -5062,7 +5147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>1</v>
       </c>
@@ -5116,7 +5201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>1</v>
       </c>
@@ -5170,7 +5255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>1</v>
       </c>
@@ -5224,7 +5309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>1</v>
       </c>
@@ -5278,7 +5363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>1</v>
       </c>
@@ -5332,7 +5417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>1</v>
       </c>
@@ -5386,7 +5471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>1</v>
       </c>
@@ -5440,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>1</v>
       </c>
@@ -5494,7 +5579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>1</v>
       </c>
@@ -5548,7 +5633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>1</v>
       </c>
@@ -5602,7 +5687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
         <v>1</v>
       </c>
@@ -5656,7 +5741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>1</v>
       </c>
@@ -5710,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>1</v>
       </c>
@@ -5764,7 +5849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>1</v>
       </c>
@@ -5818,7 +5903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>1</v>
       </c>
@@ -5872,7 +5957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>1</v>
       </c>
@@ -5926,7 +6011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>1</v>
       </c>
@@ -5980,7 +6065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>1</v>
       </c>
@@ -6034,7 +6119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>1</v>
       </c>
@@ -6088,7 +6173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
         <v>1</v>
       </c>
@@ -6142,7 +6227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="14" t="s">
         <v>1</v>
       </c>
@@ -6196,7 +6281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
         <v>1</v>
       </c>
@@ -6250,7 +6335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>1</v>
       </c>
@@ -6304,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
         <v>1</v>
       </c>
@@ -6358,7 +6443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="14" t="s">
         <v>1</v>
       </c>
@@ -6412,7 +6497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="14" t="s">
         <v>1</v>
       </c>
@@ -6466,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="14" t="s">
         <v>1</v>
       </c>
@@ -6520,7 +6605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>1</v>
       </c>
@@ -6574,7 +6659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>1</v>
       </c>
@@ -6628,7 +6713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>1</v>
       </c>
@@ -6682,7 +6767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="14" t="s">
         <v>1</v>
       </c>
@@ -6736,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>1</v>
       </c>
@@ -6790,7 +6875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>1</v>
       </c>
@@ -6844,7 +6929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="14" t="s">
         <v>1</v>
       </c>
@@ -6898,7 +6983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
         <v>1</v>
       </c>
@@ -6952,7 +7037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="14" t="s">
         <v>1</v>
       </c>
@@ -7006,7 +7091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="14" t="s">
         <v>1</v>
       </c>
@@ -7060,7 +7145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="14" t="s">
         <v>1</v>
       </c>
@@ -7114,7 +7199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="14" t="s">
         <v>1</v>
       </c>
@@ -7168,7 +7253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="14" t="s">
         <v>1</v>
       </c>
@@ -7222,7 +7307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
         <v>1</v>
       </c>
@@ -7276,7 +7361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="17" t="s">
         <v>1</v>
       </c>
@@ -7330,7 +7415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="17" t="s">
         <v>1</v>
       </c>
@@ -7384,7 +7469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="17" t="s">
         <v>1</v>
       </c>
@@ -7438,7 +7523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="17" t="s">
         <v>1</v>
       </c>
@@ -7492,7 +7577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="17" t="s">
         <v>1</v>
       </c>
@@ -7546,7 +7631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
         <v>1</v>
       </c>
@@ -7600,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
         <v>1</v>
       </c>
@@ -7654,7 +7739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="14" t="s">
         <v>1</v>
       </c>
@@ -7708,7 +7793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="14" t="s">
         <v>1</v>
       </c>
@@ -7762,7 +7847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
         <v>1</v>
       </c>
@@ -7816,7 +7901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>2</v>
       </c>
@@ -7870,7 +7955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
         <v>2</v>
       </c>
@@ -7924,7 +8009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
         <v>2</v>
       </c>
@@ -7978,7 +8063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="17" t="s">
         <v>2</v>
       </c>
@@ -8032,7 +8117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="17" t="s">
         <v>3</v>
       </c>
@@ -8086,7 +8171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="17" t="s">
         <v>2</v>
       </c>
@@ -8140,7 +8225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="17" t="s">
         <v>2</v>
       </c>
@@ -8194,7 +8279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="17" t="s">
         <v>2</v>
       </c>
@@ -8248,7 +8333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="17" t="s">
         <v>2</v>
       </c>
@@ -8302,7 +8387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="17" t="s">
         <v>2</v>
       </c>
@@ -8356,7 +8441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
         <v>4</v>
       </c>
@@ -8410,7 +8495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="17" t="s">
         <v>4</v>
       </c>
@@ -8464,7 +8549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="17" t="s">
         <v>4</v>
       </c>
@@ -8518,7 +8603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="17" t="s">
         <v>4</v>
       </c>
@@ -8572,7 +8657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="14" t="s">
         <v>4</v>
       </c>
@@ -8626,7 +8711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="17" t="s">
         <v>5</v>
       </c>
@@ -8680,7 +8765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
         <v>5</v>
       </c>
@@ -8734,7 +8819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="17" t="s">
         <v>1</v>
       </c>
@@ -8788,7 +8873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="14" t="s">
         <v>5</v>
       </c>
@@ -8842,7 +8927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="14" t="s">
         <v>5</v>
       </c>
@@ -8896,7 +8981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
         <v>5</v>
       </c>
@@ -8950,7 +9035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
         <v>5</v>
       </c>
@@ -9004,7 +9089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
         <v>5</v>
       </c>
@@ -9082,30 +9167,30 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="68.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1796875" customWidth="1"/>
-    <col min="5" max="5" width="49.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
     </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -9113,19 +9198,19 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>452</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>12</v>
       </c>
@@ -9142,7 +9227,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -9159,7 +9244,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -9173,7 +9258,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -9187,7 +9272,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -9201,7 +9286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -9215,7 +9300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -9229,7 +9314,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -9243,7 +9328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -9257,7 +9342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -9271,7 +9356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -9285,7 +9370,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -9299,7 +9384,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -9313,7 +9398,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -9327,7 +9412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -9341,7 +9426,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -9355,7 +9440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -9369,7 +9454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>110</v>
       </c>
@@ -9383,7 +9468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -9397,7 +9482,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -9411,7 +9496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -9425,7 +9510,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -9439,7 +9524,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>115</v>
       </c>
@@ -9453,7 +9538,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -9467,7 +9552,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>117</v>
       </c>
@@ -9478,7 +9563,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>118</v>
       </c>
@@ -9492,7 +9577,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -9503,7 +9588,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>120</v>
       </c>
@@ -9517,7 +9602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -9531,7 +9616,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>122</v>
       </c>
@@ -9545,7 +9630,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>123</v>
       </c>
@@ -9556,7 +9641,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>124</v>
       </c>
@@ -9567,7 +9652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>125</v>
       </c>
@@ -9578,7 +9663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>126</v>
       </c>
@@ -9592,7 +9677,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -9606,7 +9691,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>128</v>
       </c>
@@ -9620,7 +9705,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>129</v>
       </c>
@@ -9631,7 +9716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>130</v>
       </c>
@@ -9645,7 +9730,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>131</v>
       </c>
@@ -9659,7 +9744,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>132</v>
       </c>
@@ -9673,7 +9758,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -9684,7 +9769,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>134</v>
       </c>
@@ -9695,7 +9780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>135</v>
       </c>
@@ -9706,7 +9791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>136</v>
       </c>
@@ -9717,7 +9802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>137</v>
       </c>
@@ -9728,7 +9813,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>138</v>
       </c>
@@ -9739,7 +9824,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>139</v>
       </c>
@@ -9750,7 +9835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>140</v>
       </c>
@@ -9761,7 +9846,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>141</v>
       </c>
@@ -9772,7 +9857,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>142</v>
       </c>
@@ -9783,7 +9868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>143</v>
       </c>
@@ -9794,7 +9879,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>144</v>
       </c>
@@ -9805,7 +9890,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -9816,7 +9901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>146</v>
       </c>
@@ -9827,7 +9912,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>147</v>
       </c>
@@ -9838,7 +9923,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -9849,7 +9934,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>149</v>
       </c>
@@ -9860,7 +9945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -9871,7 +9956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>151</v>
       </c>
@@ -9882,7 +9967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>152</v>
       </c>
@@ -9893,7 +9978,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>153</v>
       </c>
@@ -9904,7 +9989,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -9915,7 +10000,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -9926,7 +10011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>156</v>
       </c>
@@ -9937,7 +10022,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>157</v>
       </c>
@@ -9948,7 +10033,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>158</v>
       </c>
@@ -9959,7 +10044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>159</v>
       </c>
@@ -9970,7 +10055,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>160</v>
       </c>
@@ -9981,7 +10066,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>161</v>
       </c>
@@ -9992,7 +10077,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>162</v>
       </c>
@@ -10003,7 +10088,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -10014,7 +10099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>164</v>
       </c>
@@ -10025,7 +10110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>165</v>
       </c>
@@ -10036,7 +10121,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>166</v>
       </c>
@@ -10047,7 +10132,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -10058,7 +10143,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>168</v>
       </c>
@@ -10069,7 +10154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>169</v>
       </c>
@@ -10080,7 +10165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>170</v>
       </c>
@@ -10091,7 +10176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>171</v>
       </c>
@@ -10102,7 +10187,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -10113,7 +10198,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>173</v>
       </c>
@@ -10124,7 +10209,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -10135,7 +10220,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -10146,7 +10231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>176</v>
       </c>
@@ -10157,7 +10242,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -10168,7 +10253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>178</v>
       </c>
@@ -10179,7 +10264,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>179</v>
       </c>
@@ -10190,7 +10275,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>180</v>
       </c>
@@ -10201,7 +10286,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>181</v>
       </c>
@@ -10212,7 +10297,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>182</v>
       </c>
@@ -10223,7 +10308,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -10234,7 +10319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>184</v>
       </c>
@@ -10245,7 +10330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -10256,7 +10341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>186</v>
       </c>
@@ -10267,7 +10352,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>187</v>
       </c>
@@ -10278,7 +10363,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -10289,7 +10374,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>189</v>
       </c>
@@ -10300,7 +10385,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>190</v>
       </c>
@@ -10311,7 +10396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>191</v>
       </c>
@@ -10322,7 +10407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>192</v>
       </c>
@@ -10333,7 +10418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>193</v>
       </c>
@@ -10344,7 +10429,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>194</v>
       </c>
@@ -10355,7 +10440,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>195</v>
       </c>
@@ -10366,7 +10451,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>196</v>
       </c>
@@ -10377,7 +10462,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>197</v>
       </c>
@@ -10388,7 +10473,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>198</v>
       </c>
@@ -10399,7 +10484,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>199</v>
       </c>
@@ -10410,7 +10495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>200</v>
       </c>
@@ -10421,7 +10506,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>201</v>
       </c>
@@ -10432,7 +10517,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>202</v>
       </c>
@@ -10443,7 +10528,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>203</v>
       </c>
@@ -10454,7 +10539,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>204</v>
       </c>
@@ -10465,7 +10550,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>205</v>
       </c>
@@ -10476,7 +10561,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>206</v>
       </c>
@@ -10487,7 +10572,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>207</v>
       </c>
@@ -10498,7 +10583,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>208</v>
       </c>
@@ -10509,7 +10594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>209</v>
       </c>
@@ -10520,7 +10605,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>210</v>
       </c>
@@ -10531,7 +10616,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>211</v>
       </c>
@@ -10542,7 +10627,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>212</v>
       </c>
@@ -10553,7 +10638,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>213</v>
       </c>
@@ -10564,7 +10649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>214</v>
       </c>
@@ -10575,7 +10660,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>215</v>
       </c>
@@ -10586,7 +10671,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>216</v>
       </c>
@@ -10597,7 +10682,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>217</v>
       </c>
@@ -10608,7 +10693,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>218</v>
       </c>
@@ -10619,7 +10704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>219</v>
       </c>
@@ -10630,7 +10715,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>220</v>
       </c>
@@ -10641,7 +10726,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>221</v>
       </c>
@@ -10652,7 +10737,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>222</v>
       </c>
@@ -10663,7 +10748,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>223</v>
       </c>
@@ -10674,7 +10759,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>224</v>
       </c>
@@ -10685,7 +10770,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>225</v>
       </c>
@@ -10696,7 +10781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>226</v>
       </c>
@@ -10707,7 +10792,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>451</v>
       </c>
@@ -10718,7 +10803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>227</v>
       </c>
@@ -10729,7 +10814,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>228</v>
       </c>
@@ -10740,7 +10825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>229</v>
       </c>
@@ -10751,7 +10836,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>230</v>
       </c>
@@ -10762,7 +10847,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>231</v>
       </c>
@@ -10773,7 +10858,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>232</v>
       </c>
@@ -10784,7 +10869,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>233</v>
       </c>
@@ -10795,7 +10880,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>234</v>
       </c>
@@ -10806,7 +10891,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>235</v>
       </c>
@@ -10817,7 +10902,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>236</v>
       </c>
@@ -10828,7 +10913,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>237</v>
       </c>
@@ -10839,7 +10924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>238</v>
       </c>
@@ -10850,7 +10935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>239</v>
       </c>
@@ -10861,7 +10946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>240</v>
       </c>
@@ -10872,7 +10957,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>241</v>
       </c>
@@ -10883,7 +10968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>242</v>
       </c>
@@ -10894,7 +10979,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>243</v>
       </c>
@@ -10905,7 +10990,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>244</v>
       </c>
@@ -10916,7 +11001,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>245</v>
       </c>
@@ -10927,7 +11012,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>246</v>
       </c>
@@ -10938,7 +11023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>247</v>
       </c>
@@ -10949,7 +11034,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>248</v>
       </c>
@@ -10960,7 +11045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>249</v>
       </c>
@@ -10971,7 +11056,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>250</v>
       </c>
@@ -10982,7 +11067,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>251</v>
       </c>
@@ -10993,7 +11078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>252</v>
       </c>
@@ -11004,7 +11089,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>253</v>
       </c>
@@ -11015,7 +11100,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>254</v>
       </c>
@@ -11026,7 +11111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>255</v>
       </c>
@@ -11037,7 +11122,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>256</v>
       </c>
@@ -11048,7 +11133,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>257</v>
       </c>
@@ -11059,7 +11144,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>258</v>
       </c>
@@ -11070,7 +11155,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>259</v>
       </c>
@@ -11081,7 +11166,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>260</v>
       </c>
@@ -11092,7 +11177,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>261</v>
       </c>
@@ -11103,7 +11188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>262</v>
       </c>
@@ -11114,7 +11199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>263</v>
       </c>
@@ -11125,7 +11210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C180">
         <v>60</v>
       </c>
@@ -11143,30 +11228,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2374C14-97BD-4C0C-A0B9-06A2D874015A}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
-    <col min="3" max="3" width="46.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -11174,12 +11259,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>12</v>
       </c>
@@ -11196,7 +11281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>264</v>
       </c>
@@ -11210,7 +11295,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>265</v>
       </c>
@@ -11224,7 +11309,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>266</v>
       </c>
@@ -11238,7 +11323,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>267</v>
       </c>
@@ -11252,7 +11337,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>268</v>
       </c>
@@ -11266,7 +11351,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>269</v>
       </c>
@@ -11280,7 +11365,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>270</v>
       </c>
@@ -11294,7 +11379,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>271</v>
       </c>
@@ -11308,7 +11393,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>272</v>
       </c>
@@ -11322,7 +11407,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>273</v>
       </c>
@@ -11336,7 +11421,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>274</v>
       </c>
@@ -11350,7 +11435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>275</v>
       </c>
@@ -11364,7 +11449,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>276</v>
       </c>
@@ -11378,7 +11463,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>450</v>
       </c>
@@ -11392,7 +11477,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>277</v>
       </c>
@@ -11406,7 +11491,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>278</v>
       </c>
@@ -11420,7 +11505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>279</v>
       </c>
@@ -11434,7 +11519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>280</v>
       </c>
@@ -11448,7 +11533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -11462,7 +11547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>282</v>
       </c>
@@ -11476,7 +11561,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>283</v>
       </c>
@@ -11490,7 +11575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>284</v>
       </c>
@@ -11504,7 +11589,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>285</v>
       </c>
@@ -11518,7 +11603,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>286</v>
       </c>
@@ -11532,7 +11617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>287</v>
       </c>
@@ -11546,7 +11631,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>288</v>
       </c>
@@ -11560,7 +11645,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -11574,7 +11659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>290</v>
       </c>
@@ -11588,7 +11673,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>291</v>
       </c>
@@ -11602,7 +11687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>292</v>
       </c>
@@ -11616,7 +11701,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>293</v>
       </c>
@@ -11630,7 +11715,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>294</v>
       </c>
@@ -11644,7 +11729,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>295</v>
       </c>
@@ -11658,7 +11743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>296</v>
       </c>
@@ -11672,7 +11757,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>297</v>
       </c>
@@ -11686,7 +11771,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>298</v>
       </c>
@@ -11700,7 +11785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>299</v>
       </c>
@@ -11714,7 +11799,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>300</v>
       </c>
@@ -11728,7 +11813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>301</v>
       </c>
@@ -11739,7 +11824,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>302</v>
       </c>
@@ -11750,7 +11835,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>303</v>
       </c>
@@ -11764,7 +11849,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>304</v>
       </c>
@@ -11778,7 +11863,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>305</v>
       </c>
@@ -11792,7 +11877,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>306</v>
       </c>
@@ -11806,7 +11891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>307</v>
       </c>
@@ -11820,7 +11905,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>308</v>
       </c>
@@ -11831,7 +11916,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>309</v>
       </c>
@@ -11845,7 +11930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>310</v>
       </c>
@@ -11859,7 +11944,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>311</v>
       </c>
@@ -11873,7 +11958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>312</v>
       </c>
@@ -11887,7 +11972,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>313</v>
       </c>
@@ -11901,7 +11986,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>314</v>
       </c>
@@ -11915,7 +12000,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>315</v>
       </c>
@@ -11929,7 +12014,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>316</v>
       </c>
@@ -11943,7 +12028,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>317</v>
       </c>
@@ -11957,7 +12042,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>318</v>
       </c>
@@ -11971,7 +12056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>319</v>
       </c>
@@ -11985,7 +12070,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>320</v>
       </c>
@@ -11996,7 +12081,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>321</v>
       </c>
@@ -12010,7 +12095,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>322</v>
       </c>
@@ -12021,7 +12106,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>323</v>
       </c>
@@ -12035,7 +12120,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>324</v>
       </c>
@@ -12049,7 +12134,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>325</v>
       </c>
@@ -12063,7 +12148,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>326</v>
       </c>
@@ -12077,7 +12162,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>327</v>
       </c>
@@ -12088,7 +12173,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>328</v>
       </c>
@@ -12099,7 +12184,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>329</v>
       </c>
@@ -12113,7 +12198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>330</v>
       </c>
@@ -12124,7 +12209,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>331</v>
       </c>
@@ -12138,7 +12223,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>332</v>
       </c>
@@ -12152,7 +12237,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>333</v>
       </c>
@@ -12166,7 +12251,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>334</v>
       </c>
@@ -12177,7 +12262,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>335</v>
       </c>
@@ -12191,7 +12276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>336</v>
       </c>
@@ -12205,7 +12290,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>337</v>
       </c>
@@ -12219,7 +12304,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>338</v>
       </c>
@@ -12233,7 +12318,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>339</v>
       </c>
@@ -12244,7 +12329,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>340</v>
       </c>
@@ -12255,7 +12340,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>341</v>
       </c>
@@ -12269,7 +12354,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>342</v>
       </c>
@@ -12283,7 +12368,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>343</v>
       </c>
@@ -12297,7 +12382,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>344</v>
       </c>
@@ -12311,7 +12396,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>345</v>
       </c>
@@ -12322,7 +12407,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>346</v>
       </c>
@@ -12336,7 +12421,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>347</v>
       </c>
@@ -12350,7 +12435,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>348</v>
       </c>
@@ -12364,7 +12449,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>349</v>
       </c>
@@ -12378,7 +12463,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>350</v>
       </c>
@@ -12392,7 +12477,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>351</v>
       </c>
@@ -12406,7 +12491,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>352</v>
       </c>
@@ -12420,7 +12505,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>353</v>
       </c>
@@ -12434,7 +12519,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>354</v>
       </c>
@@ -12448,7 +12533,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>355</v>
       </c>
@@ -12459,7 +12544,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>356</v>
       </c>
@@ -12473,7 +12558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>357</v>
       </c>
@@ -12484,7 +12569,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>358</v>
       </c>
@@ -12498,7 +12583,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>359</v>
       </c>
@@ -12512,7 +12597,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>360</v>
       </c>
@@ -12523,7 +12608,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>361</v>
       </c>
@@ -12534,7 +12619,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>362</v>
       </c>
@@ -12548,7 +12633,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>363</v>
       </c>
@@ -12559,7 +12644,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>364</v>
       </c>
@@ -12573,7 +12658,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>365</v>
       </c>
@@ -12584,7 +12669,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>366</v>
       </c>
@@ -12598,7 +12683,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>367</v>
       </c>
@@ -12612,7 +12697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>368</v>
       </c>
@@ -12623,7 +12708,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>369</v>
       </c>
@@ -12637,7 +12722,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>370</v>
       </c>
@@ -12648,7 +12733,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>371</v>
       </c>
@@ -12659,7 +12744,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>372</v>
       </c>
@@ -12673,7 +12758,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>373</v>
       </c>
@@ -12687,7 +12772,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>374</v>
       </c>
@@ -12698,7 +12783,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>375</v>
       </c>
@@ -12712,7 +12797,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>376</v>
       </c>
@@ -12726,7 +12811,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>377</v>
       </c>
@@ -12737,7 +12822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>378</v>
       </c>
@@ -12748,7 +12833,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -12759,7 +12844,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>380</v>
       </c>
@@ -12770,7 +12855,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>381</v>
       </c>
@@ -12784,7 +12869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>382</v>
       </c>
@@ -12798,7 +12883,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>383</v>
       </c>
@@ -12809,7 +12894,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>384</v>
       </c>
@@ -12820,7 +12905,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>385</v>
       </c>
@@ -12831,7 +12916,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>386</v>
       </c>
@@ -12842,7 +12927,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>387</v>
       </c>
@@ -12853,7 +12938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>388</v>
       </c>
@@ -12864,7 +12949,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>389</v>
       </c>
@@ -12875,7 +12960,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>390</v>
       </c>
@@ -12886,7 +12971,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>391</v>
       </c>
@@ -12897,7 +12982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>392</v>
       </c>
@@ -12908,7 +12993,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>393</v>
       </c>
@@ -12919,7 +13004,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>394</v>
       </c>
@@ -12930,7 +13015,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>395</v>
       </c>
@@ -12941,7 +13026,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>396</v>
       </c>
@@ -12952,7 +13037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>397</v>
       </c>
@@ -12963,7 +13048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>398</v>
       </c>
@@ -12974,7 +13059,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>399</v>
       </c>
@@ -12985,7 +13070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>400</v>
       </c>
@@ -12996,7 +13081,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>401</v>
       </c>
@@ -13007,7 +13092,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>402</v>
       </c>
@@ -13018,7 +13103,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>403</v>
       </c>
@@ -13029,7 +13114,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>404</v>
       </c>
@@ -13040,7 +13125,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>405</v>
       </c>
@@ -13051,7 +13136,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>406</v>
       </c>
@@ -13062,7 +13147,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>407</v>
       </c>
@@ -13073,7 +13158,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>408</v>
       </c>
@@ -13084,7 +13169,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>409</v>
       </c>
@@ -13095,7 +13180,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>410</v>
       </c>
@@ -13106,7 +13191,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>411</v>
       </c>
@@ -13117,7 +13202,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>412</v>
       </c>
@@ -13128,7 +13213,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>413</v>
       </c>
@@ -13139,7 +13224,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>414</v>
       </c>
@@ -13150,7 +13235,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>415</v>
       </c>
@@ -13161,7 +13246,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>416</v>
       </c>
@@ -13172,7 +13257,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>417</v>
       </c>
@@ -13183,7 +13268,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>418</v>
       </c>
@@ -13194,7 +13279,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>419</v>
       </c>
@@ -13205,7 +13290,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>420</v>
       </c>
@@ -13216,7 +13301,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>421</v>
       </c>
@@ -13227,7 +13312,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>422</v>
       </c>
@@ -13238,7 +13323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>423</v>
       </c>
@@ -13249,7 +13334,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>424</v>
       </c>
@@ -13260,7 +13345,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>425</v>
       </c>
@@ -13271,7 +13356,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>426</v>
       </c>
@@ -13282,7 +13367,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>427</v>
       </c>
@@ -13293,7 +13378,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>428</v>
       </c>
@@ -13304,7 +13389,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>429</v>
       </c>
@@ -13315,7 +13400,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>430</v>
       </c>
@@ -13326,7 +13411,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>431</v>
       </c>
@@ -13337,7 +13422,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>432</v>
       </c>
@@ -13348,7 +13433,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>433</v>
       </c>
@@ -13359,7 +13444,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>434</v>
       </c>
@@ -13370,7 +13455,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>435</v>
       </c>
@@ -13381,7 +13466,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>436</v>
       </c>
@@ -13392,7 +13477,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>437</v>
       </c>
@@ -13403,7 +13488,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>438</v>
       </c>
@@ -13414,7 +13499,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>439</v>
       </c>
@@ -13425,7 +13510,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>440</v>
       </c>
@@ -13436,7 +13521,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>441</v>
       </c>
@@ -13447,7 +13532,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>442</v>
       </c>
@@ -13458,7 +13543,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>443</v>
       </c>
@@ -13469,7 +13554,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>444</v>
       </c>
@@ -13480,7 +13565,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>445</v>
       </c>
@@ -13491,7 +13576,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>446</v>
       </c>
@@ -13502,7 +13587,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>447</v>
       </c>
@@ -13513,7 +13598,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>448</v>
       </c>
@@ -13524,7 +13609,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>449</v>
       </c>
@@ -13535,7 +13620,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="31"/>
       <c r="B196" s="31"/>
       <c r="C196" s="31"/>
@@ -13547,4 +13632,52 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4483405-5FFC-4EDD-902E-75E3FB56B872}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
+        <v>454</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>455</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>457</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>458</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{A198DCAD-25FD-4DA1-99C6-730376022561}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>